<commit_message>
big push... it's crowning!!!
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\R\ETC3250\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F12753ED-3F84-4EB3-A1D0-78AD842CCAC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77945D05-A295-4019-AEB0-3A2CD09AB822}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1076F1D-B98B-4D4B-9739-2B33D96DF351}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>